<commit_message>
Removed unused functions from the following classes
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/testdata.xlsx
+++ b/src/main/resources/TestData/testdata.xlsx
@@ -77,7 +77,7 @@
     <t xml:space="preserve">run</t>
   </si>
   <si>
-    <t xml:space="preserve">Cook,Bedroom,Bathroom,2,1,2,No repeat Every day Every week Every month</t>
+    <t xml:space="preserve">Cook,Bedroom,Bathroom,2,1,2,Every week  Every day  No repeat  Every month</t>
   </si>
 </sst>
 </file>
@@ -209,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,10 +240,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -410,10 +406,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.04"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
@@ -433,7 +432,7 @@
       <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reformatting and removed unused methods
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/testdata.xlsx
+++ b/src/main/resources/TestData/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Parameters</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t xml:space="preserve">com.example.day35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automationName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
   </si>
   <si>
     <t xml:space="preserve">Test Case Name</t>
@@ -319,10 +325,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,6 +391,14 @@
       </c>
       <c r="B7" s="5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -405,35 +419,35 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>